<commit_message>
SMTI form naming convention is correct
Next update: see if upload can be done automatically, excel file download, modify db
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-580</v>
+        <v>-584</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>-32</v>
+        <v>-36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>